<commit_message>
added the numbers for run2
</commit_message>
<xml_diff>
--- a/Results/ScenarioI/ScenarioI.xlsx
+++ b/Results/ScenarioI/ScenarioI.xlsx
@@ -97,10 +97,10 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Good" xfId="1" builtinId="26"/>
@@ -405,8 +405,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:K68"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D18" sqref="D18"/>
+    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="D20" sqref="D20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -418,123 +418,123 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="B1" s="2"/>
-      <c r="C1" s="2"/>
-      <c r="D1" s="2"/>
-      <c r="E1" s="2"/>
-      <c r="F1" s="2"/>
-      <c r="G1" s="2"/>
-      <c r="H1" s="2"/>
-      <c r="I1" s="2"/>
-      <c r="J1" s="2"/>
-      <c r="K1" s="2"/>
+      <c r="A1" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="B1" s="3"/>
+      <c r="C1" s="3"/>
+      <c r="D1" s="3"/>
+      <c r="E1" s="3"/>
+      <c r="F1" s="3"/>
+      <c r="G1" s="3"/>
+      <c r="H1" s="3"/>
+      <c r="I1" s="3"/>
+      <c r="J1" s="3"/>
+      <c r="K1" s="3"/>
     </row>
     <row r="2" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A2" s="2"/>
-      <c r="B2" s="2"/>
-      <c r="C2" s="2"/>
-      <c r="D2" s="2"/>
-      <c r="E2" s="2"/>
-      <c r="F2" s="2"/>
-      <c r="G2" s="2"/>
-      <c r="H2" s="2"/>
-      <c r="I2" s="2"/>
-      <c r="J2" s="2"/>
-      <c r="K2" s="2"/>
+      <c r="A2" s="3"/>
+      <c r="B2" s="3"/>
+      <c r="C2" s="3"/>
+      <c r="D2" s="3"/>
+      <c r="E2" s="3"/>
+      <c r="F2" s="3"/>
+      <c r="G2" s="3"/>
+      <c r="H2" s="3"/>
+      <c r="I2" s="3"/>
+      <c r="J2" s="3"/>
+      <c r="K2" s="3"/>
     </row>
     <row r="3" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A3" s="2"/>
-      <c r="B3" s="2"/>
-      <c r="C3" s="2"/>
-      <c r="D3" s="2"/>
-      <c r="E3" s="2"/>
-      <c r="F3" s="2"/>
-      <c r="G3" s="2"/>
-      <c r="H3" s="2"/>
-      <c r="I3" s="2"/>
-      <c r="J3" s="2"/>
-      <c r="K3" s="2"/>
+      <c r="A3" s="3"/>
+      <c r="B3" s="3"/>
+      <c r="C3" s="3"/>
+      <c r="D3" s="3"/>
+      <c r="E3" s="3"/>
+      <c r="F3" s="3"/>
+      <c r="G3" s="3"/>
+      <c r="H3" s="3"/>
+      <c r="I3" s="3"/>
+      <c r="J3" s="3"/>
+      <c r="K3" s="3"/>
     </row>
     <row r="4" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A4" s="2"/>
-      <c r="B4" s="2"/>
-      <c r="C4" s="2"/>
-      <c r="D4" s="2"/>
-      <c r="E4" s="2"/>
-      <c r="F4" s="2"/>
-      <c r="G4" s="2"/>
-      <c r="H4" s="2"/>
-      <c r="I4" s="2"/>
-      <c r="J4" s="2"/>
-      <c r="K4" s="2"/>
+      <c r="A4" s="3"/>
+      <c r="B4" s="3"/>
+      <c r="C4" s="3"/>
+      <c r="D4" s="3"/>
+      <c r="E4" s="3"/>
+      <c r="F4" s="3"/>
+      <c r="G4" s="3"/>
+      <c r="H4" s="3"/>
+      <c r="I4" s="3"/>
+      <c r="J4" s="3"/>
+      <c r="K4" s="3"/>
     </row>
     <row r="5" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A5" s="2"/>
-      <c r="B5" s="2"/>
-      <c r="C5" s="2"/>
-      <c r="D5" s="2"/>
-      <c r="E5" s="2"/>
-      <c r="F5" s="2"/>
-      <c r="G5" s="2"/>
-      <c r="H5" s="2"/>
-      <c r="I5" s="2"/>
-      <c r="J5" s="2"/>
-      <c r="K5" s="2"/>
+      <c r="A5" s="3"/>
+      <c r="B5" s="3"/>
+      <c r="C5" s="3"/>
+      <c r="D5" s="3"/>
+      <c r="E5" s="3"/>
+      <c r="F5" s="3"/>
+      <c r="G5" s="3"/>
+      <c r="H5" s="3"/>
+      <c r="I5" s="3"/>
+      <c r="J5" s="3"/>
+      <c r="K5" s="3"/>
     </row>
     <row r="6" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A6" s="2"/>
-      <c r="B6" s="2"/>
-      <c r="C6" s="2"/>
-      <c r="D6" s="2"/>
-      <c r="E6" s="2"/>
-      <c r="F6" s="2"/>
-      <c r="G6" s="2"/>
-      <c r="H6" s="2"/>
-      <c r="I6" s="2"/>
-      <c r="J6" s="2"/>
-      <c r="K6" s="2"/>
+      <c r="A6" s="3"/>
+      <c r="B6" s="3"/>
+      <c r="C6" s="3"/>
+      <c r="D6" s="3"/>
+      <c r="E6" s="3"/>
+      <c r="F6" s="3"/>
+      <c r="G6" s="3"/>
+      <c r="H6" s="3"/>
+      <c r="I6" s="3"/>
+      <c r="J6" s="3"/>
+      <c r="K6" s="3"/>
     </row>
     <row r="7" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A7" s="2"/>
-      <c r="B7" s="2"/>
-      <c r="C7" s="2"/>
-      <c r="D7" s="2"/>
-      <c r="E7" s="2"/>
-      <c r="F7" s="2"/>
-      <c r="G7" s="2"/>
-      <c r="H7" s="2"/>
-      <c r="I7" s="2"/>
-      <c r="J7" s="2"/>
-      <c r="K7" s="2"/>
+      <c r="A7" s="3"/>
+      <c r="B7" s="3"/>
+      <c r="C7" s="3"/>
+      <c r="D7" s="3"/>
+      <c r="E7" s="3"/>
+      <c r="F7" s="3"/>
+      <c r="G7" s="3"/>
+      <c r="H7" s="3"/>
+      <c r="I7" s="3"/>
+      <c r="J7" s="3"/>
+      <c r="K7" s="3"/>
     </row>
     <row r="8" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A8" s="2"/>
-      <c r="B8" s="2"/>
-      <c r="C8" s="2"/>
-      <c r="D8" s="2"/>
-      <c r="E8" s="2"/>
-      <c r="F8" s="2"/>
-      <c r="G8" s="2"/>
-      <c r="H8" s="2"/>
-      <c r="I8" s="2"/>
-      <c r="J8" s="2"/>
-      <c r="K8" s="2"/>
+      <c r="A8" s="3"/>
+      <c r="B8" s="3"/>
+      <c r="C8" s="3"/>
+      <c r="D8" s="3"/>
+      <c r="E8" s="3"/>
+      <c r="F8" s="3"/>
+      <c r="G8" s="3"/>
+      <c r="H8" s="3"/>
+      <c r="I8" s="3"/>
+      <c r="J8" s="3"/>
+      <c r="K8" s="3"/>
     </row>
     <row r="9" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A9" s="2"/>
-      <c r="B9" s="2"/>
-      <c r="C9" s="2"/>
-      <c r="D9" s="2"/>
-      <c r="E9" s="2"/>
-      <c r="F9" s="2"/>
-      <c r="G9" s="2"/>
-      <c r="H9" s="2"/>
-      <c r="I9" s="2"/>
-      <c r="J9" s="2"/>
-      <c r="K9" s="2"/>
+      <c r="A9" s="3"/>
+      <c r="B9" s="3"/>
+      <c r="C9" s="3"/>
+      <c r="D9" s="3"/>
+      <c r="E9" s="3"/>
+      <c r="F9" s="3"/>
+      <c r="G9" s="3"/>
+      <c r="H9" s="3"/>
+      <c r="I9" s="3"/>
+      <c r="J9" s="3"/>
+      <c r="K9" s="3"/>
     </row>
     <row r="10" spans="1:11" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10" s="1" t="s">
@@ -560,16 +560,16 @@
       </c>
     </row>
     <row r="11" spans="1:11" ht="30" x14ac:dyDescent="0.25">
-      <c r="A11" s="3">
+      <c r="A11" s="2">
         <v>1</v>
       </c>
-      <c r="B11" s="3">
-        <v>2</v>
-      </c>
-      <c r="C11" s="3">
-        <v>2</v>
-      </c>
-      <c r="D11" s="3">
+      <c r="B11" s="2">
+        <v>2</v>
+      </c>
+      <c r="C11" s="2">
+        <v>2</v>
+      </c>
+      <c r="D11" s="2">
         <v>1224.2</v>
       </c>
       <c r="E11" s="1">
@@ -578,7 +578,7 @@
       <c r="F11" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="G11" s="3">
+      <c r="G11" s="2">
         <v>1163.27</v>
       </c>
     </row>
@@ -753,6 +753,18 @@
       <c r="C19">
         <v>2</v>
       </c>
+      <c r="D19">
+        <v>1098.6300000000001</v>
+      </c>
+      <c r="E19">
+        <v>1098.6300000000001</v>
+      </c>
+      <c r="F19">
+        <v>982.69799999999998</v>
+      </c>
+      <c r="G19">
+        <v>1038.06</v>
+      </c>
     </row>
     <row r="20" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A20">
@@ -764,6 +776,18 @@
       <c r="C20">
         <v>2</v>
       </c>
+      <c r="D20">
+        <v>1126.78</v>
+      </c>
+      <c r="E20">
+        <v>1126.78</v>
+      </c>
+      <c r="F20">
+        <v>1054.03</v>
+      </c>
+      <c r="G20">
+        <v>1064.8800000000001</v>
+      </c>
     </row>
     <row r="22" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A22" s="1" t="s">
@@ -798,8 +822,18 @@
       <c r="C23">
         <v>2</v>
       </c>
-      <c r="E23" s="1"/>
-      <c r="F23" s="1"/>
+      <c r="D23">
+        <v>2504.63</v>
+      </c>
+      <c r="E23" s="1">
+        <v>2504.63</v>
+      </c>
+      <c r="F23" s="1">
+        <v>2298.7800000000002</v>
+      </c>
+      <c r="G23">
+        <v>2294.7399999999998</v>
+      </c>
     </row>
     <row r="24" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A24">
@@ -810,6 +844,18 @@
       </c>
       <c r="C24">
         <v>2</v>
+      </c>
+      <c r="D24">
+        <v>2556.46</v>
+      </c>
+      <c r="E24">
+        <v>2556.46</v>
+      </c>
+      <c r="F24">
+        <v>2355.91</v>
+      </c>
+      <c r="G24">
+        <v>2398.65</v>
       </c>
     </row>
     <row r="25" spans="1:7" x14ac:dyDescent="0.25">
@@ -822,6 +868,18 @@
       <c r="C25">
         <v>2</v>
       </c>
+      <c r="D25">
+        <v>2610.67</v>
+      </c>
+      <c r="E25">
+        <v>2610.67</v>
+      </c>
+      <c r="F25">
+        <v>2493.2199999999998</v>
+      </c>
+      <c r="G25">
+        <v>2426.2399999999998</v>
+      </c>
     </row>
     <row r="26" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A26">
@@ -832,6 +890,18 @@
       </c>
       <c r="C26">
         <v>2</v>
+      </c>
+      <c r="D26">
+        <v>2497.88</v>
+      </c>
+      <c r="E26">
+        <v>2497.88</v>
+      </c>
+      <c r="F26">
+        <v>2346.5700000000002</v>
+      </c>
+      <c r="G26">
+        <v>2339.84</v>
       </c>
     </row>
     <row r="27" spans="1:7" x14ac:dyDescent="0.25">
@@ -844,6 +914,18 @@
       <c r="C27">
         <v>2</v>
       </c>
+      <c r="D27">
+        <v>2626.53</v>
+      </c>
+      <c r="E27">
+        <v>2626.53</v>
+      </c>
+      <c r="F27">
+        <v>2509.63</v>
+      </c>
+      <c r="G27">
+        <v>2229.88</v>
+      </c>
     </row>
     <row r="28" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A28">
@@ -854,6 +936,18 @@
       </c>
       <c r="C28">
         <v>2</v>
+      </c>
+      <c r="D28">
+        <v>2492.1999999999998</v>
+      </c>
+      <c r="E28">
+        <v>2492.1999999999998</v>
+      </c>
+      <c r="F28">
+        <v>2374.19</v>
+      </c>
+      <c r="G28">
+        <v>2257.34</v>
       </c>
     </row>
     <row r="29" spans="1:7" x14ac:dyDescent="0.25">
@@ -866,6 +960,18 @@
       <c r="C29">
         <v>2</v>
       </c>
+      <c r="D29">
+        <v>2514.3000000000002</v>
+      </c>
+      <c r="E29">
+        <v>2514.3000000000002</v>
+      </c>
+      <c r="F29">
+        <v>2396.31</v>
+      </c>
+      <c r="G29">
+        <v>2358.08</v>
+      </c>
     </row>
     <row r="30" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A30">
@@ -876,6 +982,18 @@
       </c>
       <c r="C30">
         <v>2</v>
+      </c>
+      <c r="D30">
+        <v>2586.29</v>
+      </c>
+      <c r="E30">
+        <v>2586.29</v>
+      </c>
+      <c r="F30">
+        <v>2467.23</v>
+      </c>
+      <c r="G30">
+        <v>2330.46</v>
       </c>
     </row>
     <row r="31" spans="1:7" x14ac:dyDescent="0.25">
@@ -887,6 +1005,18 @@
       </c>
       <c r="C31">
         <v>2</v>
+      </c>
+      <c r="D31">
+        <v>2584.27</v>
+      </c>
+      <c r="E31">
+        <v>2584.27</v>
+      </c>
+      <c r="F31">
+        <v>2430.89</v>
+      </c>
+      <c r="G31">
+        <v>2451.56</v>
       </c>
     </row>
     <row r="32" spans="1:7" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
added scenario I, proto I run information
</commit_message>
<xml_diff>
--- a/Results/ScenarioI/ScenarioI.xlsx
+++ b/Results/ScenarioI/ScenarioI.xlsx
@@ -406,7 +406,7 @@
   <dimension ref="A1:K68"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="D20" sqref="D20"/>
+      <selection activeCell="E38" sqref="E38"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1028,6 +1028,18 @@
       </c>
       <c r="C32">
         <v>2</v>
+      </c>
+      <c r="D32">
+        <v>2402.23</v>
+      </c>
+      <c r="E32">
+        <v>2402.23</v>
+      </c>
+      <c r="F32">
+        <v>2220.66</v>
+      </c>
+      <c r="G32">
+        <v>2214.8200000000002</v>
       </c>
     </row>
     <row r="34" spans="1:7" ht="30" x14ac:dyDescent="0.25">

</xml_diff>